<commit_message>
add pre for transportation
</commit_message>
<xml_diff>
--- a/dataset/Transportation/cross_harbor_transportation.xlsx
+++ b/dataset/Transportation/cross_harbor_transportation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yilin/Documents/COMP7507 Visualization and Visual Analytics/final project/TravelFriendlyCity/dataset/Transportation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D65B6B8-1CDF-DE43-8A2E-2373FA11F5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12590D6-5059-184A-BFEF-78CAE6274244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="2780" windowWidth="27840" windowHeight="16940" xr2:uid="{9662742E-CC5E-9148-A207-F7DF0D6D2FBC}"/>
+    <workbookView xWindow="8000" yWindow="2780" windowWidth="27840" windowHeight="16940" xr2:uid="{9662742E-CC5E-9148-A207-F7DF0D6D2FBC}"/>
   </bookViews>
   <sheets>
     <sheet name="cross_harbor_trans" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="7">
   <si>
     <t>YR_MTH</t>
   </si>
@@ -55,6 +55,10 @@
   </si>
   <si>
     <t>Railways</t>
+  </si>
+  <si>
+    <t>PAX_PUB (thousands)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -451,15 +455,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29392FF6-4FF2-7F4C-A56D-A83CD5D0E331}">
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:D169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D169" sqref="D169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,30 +473,39 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>201901</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2">
-        <v>20187.486000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>2109.0819999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>4085.7579999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>201901</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>2109.0819999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>20187.486000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>132367.375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>201901</v>
       </c>
@@ -502,30 +515,39 @@
       <c r="C4" s="2">
         <v>39439.737999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="2">
+        <v>182906.89799999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>201902</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2">
-        <v>17394.796999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>2111.7660000000001</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4049.1210000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>201902</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>2111.7660000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>17394.796999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>114545.16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>201902</v>
       </c>
@@ -535,41 +557,53 @@
       <c r="C7" s="2">
         <v>33634.464</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="2">
+        <v>155707.69200000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>201903</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="2">
-        <v>19970.292000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>1997.3679999999999</v>
+      </c>
+      <c r="D8" s="2">
+        <v>3990.5569999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>201903</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>38123.057000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>19970.292000000001</v>
+      </c>
+      <c r="D9" s="2">
+        <v>130830.54399999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>201903</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
-        <v>1997.3679999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>38123.057000000001</v>
+      </c>
+      <c r="D10" s="2">
+        <v>178409.48699999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>201904</v>
       </c>
@@ -579,96 +613,123 @@
       <c r="C11" s="2">
         <v>1844.9949999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="2">
+        <v>3891.0830000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>201904</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>34803.305</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>18355.208999999999</v>
+      </c>
+      <c r="D12" s="2">
+        <v>122484.215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>201904</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2">
-        <v>18355.208999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>34803.305</v>
+      </c>
+      <c r="D13" s="2">
+        <v>164611.91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>201905</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="2">
-        <v>19266.234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>1831.0409999999999</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3872.0729999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>201905</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="2">
-        <v>37490.466</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>19266.234</v>
+      </c>
+      <c r="D15" s="2">
+        <v>129592.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>201905</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2">
-        <v>1831.0409999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>37490.466</v>
+      </c>
+      <c r="D16" s="2">
+        <v>175993.31099999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="2">
         <v>201906</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" s="2">
-        <v>18038.082999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>1802.1880000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>3653.085</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>201906</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>36421.025999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>18038.082999999999</v>
+      </c>
+      <c r="D18" s="2">
+        <v>123628.74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="2">
         <v>201906</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C19" s="2">
-        <v>1802.1880000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>36421.025999999998</v>
+      </c>
+      <c r="D19" s="2">
+        <v>167675.77799999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>201907</v>
       </c>
@@ -678,52 +739,67 @@
       <c r="C20" s="2">
         <v>1801.69</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="2">
+        <v>3600.3090000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2">
         <v>201907</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="2">
-        <v>36938.383999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>19071.543000000001</v>
+      </c>
+      <c r="D21" s="2">
+        <v>125941.599</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="2">
         <v>201907</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2">
-        <v>19071.543000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>36938.383999999998</v>
+      </c>
+      <c r="D22" s="2">
+        <v>169487.073</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="2">
         <v>201908</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C23" s="2">
-        <v>18361.235000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>1480.354</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3231.2109999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="2">
         <v>201908</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C24" s="2">
-        <v>1480.354</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>18361.235000000001</v>
+      </c>
+      <c r="D24" s="2">
+        <v>120975.808</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="2">
         <v>201908</v>
       </c>
@@ -733,30 +809,39 @@
       <c r="C25" s="2">
         <v>34473.642</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25" s="2">
+        <v>159684.94699999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="2">
         <v>201909</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C26" s="2">
-        <v>19170.011999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>1405.1320000000001</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3187.2930000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="2">
         <v>201909</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" s="2">
-        <v>1405.1320000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>19170.011999999999</v>
+      </c>
+      <c r="D27" s="2">
+        <v>128068.811</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="2">
         <v>201909</v>
       </c>
@@ -766,8 +851,11 @@
       <c r="C28" s="2">
         <v>32270.383000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28" s="2">
+        <v>155190.37299999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="2">
         <v>201910</v>
       </c>
@@ -777,30 +865,39 @@
       <c r="C29" s="2">
         <v>1720.836</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29" s="2">
+        <v>3560.1329999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="2">
         <v>201910</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C30" s="2">
-        <v>28515.521000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>20790.53</v>
+      </c>
+      <c r="D30" s="2">
+        <v>132205.736</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="2">
         <v>201910</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C31" s="2">
-        <v>20790.53</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>28515.521000000001</v>
+      </c>
+      <c r="D31" s="2">
+        <v>130271.353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="2">
         <v>201911</v>
       </c>
@@ -810,96 +907,123 @@
       <c r="C32" s="2">
         <v>1955.598</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="D32" s="2">
+        <v>3811.8739999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="2">
         <v>201911</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33" s="2">
-        <v>30210.698</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>14346.74</v>
+      </c>
+      <c r="D33" s="2">
+        <v>108460.844</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="2">
         <v>201911</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C34" s="2">
-        <v>14346.74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>30210.698</v>
+      </c>
+      <c r="D34" s="2">
+        <v>129743.10400000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="2">
         <v>201912</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" s="2">
-        <v>19197.323</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>1721.115</v>
+      </c>
+      <c r="D35" s="2">
+        <v>3660.431</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="2">
         <v>201912</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36" s="2">
-        <v>32448.576000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>19197.323</v>
+      </c>
+      <c r="D36" s="2">
+        <v>125181.19500000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="2">
         <v>201912</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37" s="2">
-        <v>1721.115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>32448.576000000001</v>
+      </c>
+      <c r="D37" s="2">
+        <v>147677.29699999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="2">
         <v>202001</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C38" s="2">
-        <v>17896.398000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>1506.95</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3334.684999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="2">
         <v>202001</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C39" s="2">
-        <v>29922.053</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>17896.398000000001</v>
+      </c>
+      <c r="D39" s="2">
+        <v>119633.586</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="2">
         <v>202001</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" s="2">
-        <v>1506.95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>29922.053</v>
+      </c>
+      <c r="D40" s="2">
+        <v>140402.50200000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="2">
         <v>202002</v>
       </c>
@@ -909,63 +1033,81 @@
       <c r="C41" s="2">
         <v>783.16200000000003</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="2">
+        <v>2094.7840000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="2">
         <v>202002</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2">
-        <v>17998.593000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>11617.346</v>
+      </c>
+      <c r="D42" s="2">
+        <v>73687.516999999993</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="2">
         <v>202002</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C43" s="2">
-        <v>11617.346</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>17998.593000000001</v>
+      </c>
+      <c r="D43" s="2">
+        <v>81420.436000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="2">
         <v>202003</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="2">
-        <v>13339.794</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>885.89499999999998</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2394.7669999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="2">
         <v>202003</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C45" s="2">
-        <v>21318.455000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>13339.794</v>
+      </c>
+      <c r="D45" s="2">
+        <v>82060.556000000011</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="2">
         <v>202003</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46" s="2">
-        <v>885.89499999999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>21318.455000000002</v>
+      </c>
+      <c r="D46" s="2">
+        <v>95358.843999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="2">
         <v>202004</v>
       </c>
@@ -975,63 +1117,81 @@
       <c r="C47" s="2">
         <v>819.03499999999997</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
+      <c r="D47" s="2">
+        <v>2243.221</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="2">
         <v>202004</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C48" s="2">
-        <v>18165.293000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>11742.942999999999</v>
+      </c>
+      <c r="D48" s="2">
+        <v>74655.704999999987</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="2">
         <v>202004</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C49" s="2">
-        <v>11742.942999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>18165.293000000001</v>
+      </c>
+      <c r="D49" s="2">
+        <v>85130.130999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="2">
         <v>202005</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C50" s="2">
-        <v>14954.638999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>1041.345</v>
+      </c>
+      <c r="D50" s="2">
+        <v>2804.328</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="2">
         <v>202005</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2">
-        <v>24542.14</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>14954.638999999999</v>
+      </c>
+      <c r="D51" s="2">
+        <v>94298.412999999986</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52" s="2">
         <v>202005</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" s="2">
-        <v>1041.345</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>24542.14</v>
+      </c>
+      <c r="D52" s="2">
+        <v>110109.709</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" s="2">
         <v>202006</v>
       </c>
@@ -1041,8 +1201,11 @@
       <c r="C53" s="2">
         <v>1043.8720000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
+      <c r="D53" s="2">
+        <v>2821.165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54" s="2">
         <v>202006</v>
       </c>
@@ -1052,8 +1215,11 @@
       <c r="C54" s="2">
         <v>16242.76</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
+      <c r="D54" s="2">
+        <v>104919.522</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55" s="2">
         <v>202006</v>
       </c>
@@ -1063,8 +1229,11 @@
       <c r="C55" s="2">
         <v>27679.629000000001</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
+      <c r="D55" s="2">
+        <v>124969.393</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
       <c r="A56" s="2">
         <v>202007</v>
       </c>
@@ -1074,30 +1243,39 @@
       <c r="C56" s="2">
         <v>844.24399999999991</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
+      <c r="D56" s="2">
+        <v>2333.462</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
       <c r="A57" s="2">
         <v>202007</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C57" s="2">
-        <v>23183.628000000001</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>13712.905000000001</v>
+      </c>
+      <c r="D57" s="2">
+        <v>88706.34599999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
       <c r="A58" s="2">
         <v>202007</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C58" s="2">
-        <v>13712.905000000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>23183.628000000001</v>
+      </c>
+      <c r="D58" s="2">
+        <v>103675.315</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
       <c r="A59" s="2">
         <v>202008</v>
       </c>
@@ -1107,30 +1285,39 @@
       <c r="C59" s="2">
         <v>715.52800000000002</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
+      <c r="D59" s="2">
+        <v>2045.43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
       <c r="A60" s="2">
         <v>202008</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C60" s="2">
-        <v>19348.851999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>11819.636</v>
+      </c>
+      <c r="D60" s="2">
+        <v>76840.183000000005</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
       <c r="A61" s="2">
         <v>202008</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C61" s="2">
-        <v>11819.636</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>19348.851999999999</v>
+      </c>
+      <c r="D61" s="2">
+        <v>89537.654999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
       <c r="A62" s="2">
         <v>202009</v>
       </c>
@@ -1140,8 +1327,11 @@
       <c r="C62" s="2">
         <v>871.83200000000011</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
+      <c r="D62" s="2">
+        <v>2410.7669999999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
       <c r="A63" s="2">
         <v>202009</v>
       </c>
@@ -1151,8 +1341,11 @@
       <c r="C63" s="2">
         <v>14627.669</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
+      <c r="D63" s="2">
+        <v>94382.926000000007</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
       <c r="A64" s="2">
         <v>202009</v>
       </c>
@@ -1162,41 +1355,53 @@
       <c r="C64" s="2">
         <v>25505.374</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
+      <c r="D64" s="2">
+        <v>114442.61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
       <c r="A65" s="2">
         <v>202010</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C65" s="2">
-        <v>15857.981</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>1127.0250000000001</v>
+      </c>
+      <c r="D65" s="2">
+        <v>3201.645</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
       <c r="A66" s="2">
         <v>202010</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C66" s="2">
-        <v>28132.073</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>15857.981</v>
+      </c>
+      <c r="D66" s="2">
+        <v>106463.59299999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
       <c r="A67" s="2">
         <v>202010</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C67" s="2">
-        <v>1127.0250000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>28132.073</v>
+      </c>
+      <c r="D67" s="2">
+        <v>129301.745</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
       <c r="A68" s="2">
         <v>202011</v>
       </c>
@@ -1206,85 +1411,109 @@
       <c r="C68" s="2">
         <v>1131.403</v>
       </c>
-    </row>
-    <row r="69" spans="1:3">
+      <c r="D68" s="2">
+        <v>3033.627</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
       <c r="A69" s="2">
         <v>202011</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C69" s="2">
-        <v>28675.946</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <v>16243.348</v>
+      </c>
+      <c r="D69" s="2">
+        <v>106846.15300000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
       <c r="A70" s="2">
         <v>202011</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C70" s="2">
-        <v>16243.348</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <v>28675.946</v>
+      </c>
+      <c r="D70" s="2">
+        <v>129932.973</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
       <c r="A71" s="2">
         <v>202012</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C71" s="2">
-        <v>13448.566000000001</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <v>1053.8510000000001</v>
+      </c>
+      <c r="D71" s="2">
+        <v>2725.0819999999999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
       <c r="A72" s="2">
         <v>202012</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C72" s="2">
-        <v>22831.243999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <v>13448.566000000001</v>
+      </c>
+      <c r="D72" s="2">
+        <v>88776.054999999993</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
       <c r="A73" s="2">
         <v>202012</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C73" s="2">
-        <v>1053.8510000000001</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <v>22831.243999999999</v>
+      </c>
+      <c r="D73" s="2">
+        <v>105864.633</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
       <c r="A74" s="2">
         <v>202101</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C74" s="2">
-        <v>13482.781999999999</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>896.71799999999985</v>
+      </c>
+      <c r="D74" s="2">
+        <v>2529.2240000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
       <c r="A75" s="2">
         <v>202101</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C75" s="2">
-        <v>896.71799999999985</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <v>13482.781999999999</v>
+      </c>
+      <c r="D75" s="2">
+        <v>88286.856</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
       <c r="A76" s="2">
         <v>202101</v>
       </c>
@@ -1294,30 +1523,39 @@
       <c r="C76" s="2">
         <v>23030.526999999998</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
+      <c r="D76" s="2">
+        <v>106090.78</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
       <c r="A77" s="2">
         <v>202102</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C77" s="2">
-        <v>12970.130999999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <v>972.07600000000002</v>
+      </c>
+      <c r="D77" s="2">
+        <v>2839.5720000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
       <c r="A78" s="2">
         <v>202102</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C78" s="2">
-        <v>972.07600000000002</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <v>12970.130999999999</v>
+      </c>
+      <c r="D78" s="2">
+        <v>85489.21</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
       <c r="A79" s="2">
         <v>202102</v>
       </c>
@@ -1327,8 +1565,11 @@
       <c r="C79" s="2">
         <v>22494.489000000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
+      <c r="D79" s="2">
+        <v>104057.742</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
       <c r="A80" s="2">
         <v>202103</v>
       </c>
@@ -1338,85 +1579,109 @@
       <c r="C80" s="2">
         <v>1067.546</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
+      <c r="D80" s="2">
+        <v>2983.9090000000001</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
       <c r="A81" s="2">
         <v>202103</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C81" s="2">
-        <v>28512.449000000001</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <v>16352.267</v>
+      </c>
+      <c r="D81" s="2">
+        <v>105060.504</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
       <c r="A82" s="2">
         <v>202103</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C82" s="2">
-        <v>16352.267</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <v>28512.449000000001</v>
+      </c>
+      <c r="D82" s="2">
+        <v>129953.84699999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
       <c r="A83" s="2">
         <v>202104</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C83" s="2">
-        <v>16126.468999999999</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <v>1147.6559999999999</v>
+      </c>
+      <c r="D83" s="2">
+        <v>3261.3850000000002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
       <c r="A84" s="2">
         <v>202104</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C84" s="2">
-        <v>27568.727999999999</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <v>16126.468999999999</v>
+      </c>
+      <c r="D84" s="2">
+        <v>104673.272</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
       <c r="A85" s="2">
         <v>202104</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C85" s="2">
-        <v>1147.6559999999999</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <v>27568.727999999999</v>
+      </c>
+      <c r="D85" s="2">
+        <v>126393.88099999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
       <c r="A86" s="2">
         <v>202105</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C86" s="2">
-        <v>16760.259999999998</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <v>1031.6179999999999</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2901.8049999999998</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
       <c r="A87" s="2">
         <v>202105</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C87" s="2">
-        <v>1031.6179999999999</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <v>16760.259999999998</v>
+      </c>
+      <c r="D87" s="2">
+        <v>110158.825</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
       <c r="A88" s="2">
         <v>202105</v>
       </c>
@@ -1426,74 +1691,95 @@
       <c r="C88" s="2">
         <v>28784.620999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
+      <c r="D88" s="2">
+        <v>134398.45000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
       <c r="A89" s="2">
         <v>202106</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89" s="2">
-        <v>29149.769</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <v>1001.787</v>
+      </c>
+      <c r="D89" s="2">
+        <v>2697.2089999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
       <c r="A90" s="2">
         <v>202106</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90" s="2">
-        <v>1001.787</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+        <v>16257.29</v>
+      </c>
+      <c r="D90" s="2">
+        <v>107750.632</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
       <c r="A91" s="2">
         <v>202106</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C91" s="2">
-        <v>16257.29</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <v>29149.769</v>
+      </c>
+      <c r="D91" s="2">
+        <v>134382.95199999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
       <c r="A92" s="2">
         <v>202107</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C92" s="2">
-        <v>16869.839</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <v>1128.6590000000001</v>
+      </c>
+      <c r="D92" s="2">
+        <v>2962.6350000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
       <c r="A93" s="2">
         <v>202107</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C93" s="2">
-        <v>30936.307000000001</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <v>16869.839</v>
+      </c>
+      <c r="D93" s="2">
+        <v>109234.837</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
       <c r="A94" s="2">
         <v>202107</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C94" s="2">
-        <v>1128.6590000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <v>30936.307000000001</v>
+      </c>
+      <c r="D94" s="2">
+        <v>142383.47700000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
       <c r="A95" s="2">
         <v>202108</v>
       </c>
@@ -1503,52 +1789,67 @@
       <c r="C95" s="2">
         <v>1148.231</v>
       </c>
-    </row>
-    <row r="96" spans="1:3">
+      <c r="D95" s="2">
+        <v>3051.375</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
       <c r="A96" s="2">
         <v>202108</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C96" s="2">
-        <v>31379.347000000002</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+        <v>17079.605</v>
+      </c>
+      <c r="D96" s="2">
+        <v>110067.95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
       <c r="A97" s="2">
         <v>202108</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C97" s="2">
-        <v>17079.605</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <v>31379.347000000002</v>
+      </c>
+      <c r="D97" s="2">
+        <v>144504.62700000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
       <c r="A98" s="2">
         <v>202109</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C98" s="2">
-        <v>16928.295999999998</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <v>1000.654</v>
+      </c>
+      <c r="D98" s="2">
+        <v>2784.36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
       <c r="A99" s="2">
         <v>202109</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C99" s="2">
-        <v>1000.654</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+        <v>16928.295999999998</v>
+      </c>
+      <c r="D99" s="2">
+        <v>112871.376</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
       <c r="A100" s="2">
         <v>202109</v>
       </c>
@@ -1558,8 +1859,11 @@
       <c r="C100" s="2">
         <v>31040.329000000002</v>
       </c>
-    </row>
-    <row r="101" spans="1:3">
+      <c r="D100" s="2">
+        <v>147095.03599999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
       <c r="A101" s="2">
         <v>202110</v>
       </c>
@@ -1569,63 +1873,81 @@
       <c r="C101" s="2">
         <v>1005.876</v>
       </c>
-    </row>
-    <row r="102" spans="1:3">
+      <c r="D101" s="2">
+        <v>2803.0320000000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
       <c r="A102" s="2">
         <v>202110</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C102" s="2">
-        <v>29841.870999999999</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <v>15786.362999999999</v>
+      </c>
+      <c r="D102" s="2">
+        <v>105694.539</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
       <c r="A103" s="2">
         <v>202110</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C103" s="2">
-        <v>15786.362999999999</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <v>29841.870999999999</v>
+      </c>
+      <c r="D103" s="2">
+        <v>141732.791</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
       <c r="A104" s="2">
         <v>202111</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C104" s="2">
-        <v>17576.968000000001</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <v>1155.617</v>
+      </c>
+      <c r="D104" s="2">
+        <v>3165.357</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
       <c r="A105" s="2">
         <v>202111</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C105" s="2">
-        <v>32057.85</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <v>17576.968000000001</v>
+      </c>
+      <c r="D105" s="2">
+        <v>114078.519</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
       <c r="A106" s="2">
         <v>202111</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C106" s="2">
-        <v>1155.617</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <v>32057.85</v>
+      </c>
+      <c r="D106" s="2">
+        <v>149049.88099999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
       <c r="A107" s="2">
         <v>202112</v>
       </c>
@@ -1635,52 +1957,67 @@
       <c r="C107" s="2">
         <v>1459.278</v>
       </c>
-    </row>
-    <row r="108" spans="1:3">
+      <c r="D107" s="2">
+        <v>3524.5479999999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
       <c r="A108" s="2">
         <v>202112</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C108" s="2">
-        <v>33080.644</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <v>18179.554</v>
+      </c>
+      <c r="D108" s="2">
+        <v>113673.351</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
       <c r="A109" s="2">
         <v>202112</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C109" s="2">
-        <v>18179.554</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <v>33080.644</v>
+      </c>
+      <c r="D109" s="2">
+        <v>153809.853</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
       <c r="A110" s="2">
         <v>202201</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C110" s="2">
-        <v>14831.1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <v>894.01299999999992</v>
+      </c>
+      <c r="D110" s="2">
+        <v>2521.41</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
       <c r="A111" s="2">
         <v>202201</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C111" s="2">
-        <v>894.01299999999992</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <v>14831.1</v>
+      </c>
+      <c r="D111" s="2">
+        <v>97936.213000000003</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
       <c r="A112" s="2">
         <v>202201</v>
       </c>
@@ -1690,30 +2027,39 @@
       <c r="C112" s="2">
         <v>26060.098000000002</v>
       </c>
-    </row>
-    <row r="113" spans="1:3">
+      <c r="D112" s="2">
+        <v>125070.87699999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
       <c r="A113" s="2">
         <v>202202</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C113" s="2">
-        <v>8792.44</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
+        <v>523.72400000000005</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1601.913</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
       <c r="A114" s="2">
         <v>202202</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C114" s="2">
-        <v>523.72400000000005</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
+        <v>8792.44</v>
+      </c>
+      <c r="D114" s="2">
+        <v>58044.885999999999</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
       <c r="A115" s="2">
         <v>202202</v>
       </c>
@@ -1723,30 +2069,39 @@
       <c r="C115" s="2">
         <v>14534.834999999999</v>
       </c>
-    </row>
-    <row r="116" spans="1:3">
+      <c r="D115" s="2">
+        <v>71867.035000000003</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
       <c r="A116" s="2">
         <v>202203</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C116" s="2">
-        <v>9338.1020000000008</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
+        <v>364.77499999999998</v>
+      </c>
+      <c r="D116" s="2">
+        <v>1456.4739999999999</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
       <c r="A117" s="2">
         <v>202203</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C117" s="2">
-        <v>364.77499999999998</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
+        <v>9338.1020000000008</v>
+      </c>
+      <c r="D117" s="2">
+        <v>57666.49700000001</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
       <c r="A118" s="2">
         <v>202203</v>
       </c>
@@ -1756,30 +2111,39 @@
       <c r="C118" s="2">
         <v>14837.136</v>
       </c>
-    </row>
-    <row r="119" spans="1:3">
+      <c r="D118" s="2">
+        <v>74467.438999999998</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
       <c r="A119" s="2">
         <v>202204</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C119" s="2">
-        <v>12973.696</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
+        <v>812.6400000000001</v>
+      </c>
+      <c r="D119" s="2">
+        <v>2800.6559999999999</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
       <c r="A120" s="2">
         <v>202204</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120" s="2">
-        <v>812.6400000000001</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
+        <v>12973.696</v>
+      </c>
+      <c r="D120" s="2">
+        <v>80733.114999999991</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
       <c r="A121" s="2">
         <v>202204</v>
       </c>
@@ -1789,74 +2153,95 @@
       <c r="C121" s="2">
         <v>21086.294999999998</v>
       </c>
-    </row>
-    <row r="122" spans="1:3">
+      <c r="D121" s="2">
+        <v>103309.442</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
       <c r="A122" s="2">
         <v>202205</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C122" s="2">
-        <v>14995.383</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
+        <v>877.74699999999996</v>
+      </c>
+      <c r="D122" s="2">
+        <v>2675.6590000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
       <c r="A123" s="2">
         <v>202205</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C123" s="2">
-        <v>29035.152999999998</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
+        <v>14995.383</v>
+      </c>
+      <c r="D123" s="2">
+        <v>100167.61900000001</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
       <c r="A124" s="2">
         <v>202205</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C124" s="2">
-        <v>877.74699999999996</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
+        <v>29035.152999999998</v>
+      </c>
+      <c r="D124" s="2">
+        <v>135674.603</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
       <c r="A125" s="2">
         <v>202206</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C125" s="2">
-        <v>14449.589</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
+        <v>798.76600000000008</v>
+      </c>
+      <c r="D125" s="2">
+        <v>2492.9810000000002</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
       <c r="A126" s="2">
         <v>202206</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C126" s="2">
-        <v>30603.561000000002</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
+        <v>14449.589</v>
+      </c>
+      <c r="D126" s="2">
+        <v>101557.78</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
       <c r="A127" s="2">
         <v>202206</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C127" s="2">
-        <v>798.76600000000008</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
+        <v>30603.561000000002</v>
+      </c>
+      <c r="D127" s="2">
+        <v>137826.546</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
       <c r="A128" s="2">
         <v>202207</v>
       </c>
@@ -1866,8 +2251,11 @@
       <c r="C128" s="2">
         <v>899.9190000000001</v>
       </c>
-    </row>
-    <row r="129" spans="1:3">
+      <c r="D128" s="2">
+        <v>2510.1909999999998</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
       <c r="A129" s="2">
         <v>202207</v>
       </c>
@@ -1877,8 +2265,11 @@
       <c r="C129" s="2">
         <v>14458.013000000001</v>
       </c>
-    </row>
-    <row r="130" spans="1:3">
+      <c r="D129" s="2">
+        <v>102004.47</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
       <c r="A130" s="2">
         <v>202207</v>
       </c>
@@ -1888,30 +2279,39 @@
       <c r="C130" s="2">
         <v>31203.94</v>
       </c>
-    </row>
-    <row r="131" spans="1:3">
+      <c r="D130" s="2">
+        <v>139166.29300000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
       <c r="A131" s="2">
         <v>202208</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C131" s="2">
-        <v>14799.107</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
+        <v>825.428</v>
+      </c>
+      <c r="D131" s="2">
+        <v>2533.4989999999998</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
       <c r="A132" s="2">
         <v>202208</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C132" s="2">
-        <v>825.428</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
+        <v>14799.107</v>
+      </c>
+      <c r="D132" s="2">
+        <v>103775.27099999999</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
       <c r="A133" s="2">
         <v>202208</v>
       </c>
@@ -1921,8 +2321,11 @@
       <c r="C133" s="2">
         <v>32580.84</v>
       </c>
-    </row>
-    <row r="134" spans="1:3">
+      <c r="D133" s="2">
+        <v>143012.6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
       <c r="A134" s="2">
         <v>202209</v>
       </c>
@@ -1932,85 +2335,109 @@
       <c r="C134" s="2">
         <v>818.58699999999999</v>
       </c>
-    </row>
-    <row r="135" spans="1:3">
+      <c r="D134" s="2">
+        <v>2567.953</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
       <c r="A135" s="2">
         <v>202209</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C135" s="2">
-        <v>31849.385999999999</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
+        <v>14785.874</v>
+      </c>
+      <c r="D135" s="2">
+        <v>106729.413</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
       <c r="A136" s="2">
         <v>202209</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C136" s="2">
-        <v>14785.874</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
+        <v>31849.385999999999</v>
+      </c>
+      <c r="D136" s="2">
+        <v>143678.731</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
       <c r="A137" s="2">
         <v>202210</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C137" s="2">
-        <v>15470.636</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
+        <v>947.673</v>
+      </c>
+      <c r="D137" s="2">
+        <v>2971.4090000000001</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
       <c r="A138" s="2">
         <v>202210</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C138" s="2">
-        <v>33029.048000000003</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
+        <v>15470.636</v>
+      </c>
+      <c r="D138" s="2">
+        <v>111642.836</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
       <c r="A139" s="2">
         <v>202210</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C139" s="2">
-        <v>947.673</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
+        <v>33029.048000000003</v>
+      </c>
+      <c r="D139" s="2">
+        <v>148942.15100000001</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
       <c r="A140" s="2">
         <v>202211</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C140" s="2">
-        <v>14952.695</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
+        <v>894.7639999999999</v>
+      </c>
+      <c r="D140" s="2">
+        <v>2715.7440000000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
       <c r="A141" s="2">
         <v>202211</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141" s="2">
-        <v>894.7639999999999</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+        <v>14952.695</v>
+      </c>
+      <c r="D141" s="2">
+        <v>106518.992</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
       <c r="A142" s="2">
         <v>202211</v>
       </c>
@@ -2020,30 +2447,39 @@
       <c r="C142" s="2">
         <v>32452.6</v>
       </c>
-    </row>
-    <row r="143" spans="1:3">
+      <c r="D142" s="2">
+        <v>143487.73000000001</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
       <c r="A143" s="2">
         <v>202212</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C143" s="2">
-        <v>15262.509</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
+        <v>1163.8589999999999</v>
+      </c>
+      <c r="D143" s="2">
+        <v>3104.462</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
       <c r="A144" s="2">
         <v>202212</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C144" s="2">
-        <v>1163.8589999999999</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3">
+        <v>15262.509</v>
+      </c>
+      <c r="D144" s="2">
+        <v>106721.57</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
       <c r="A145" s="2">
         <v>202212</v>
       </c>
@@ -2053,63 +2489,81 @@
       <c r="C145" s="2">
         <v>32870.919000000002</v>
       </c>
-    </row>
-    <row r="146" spans="1:3">
+      <c r="D145" s="2">
+        <v>145891.182</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
       <c r="A146" s="2">
         <v>202301</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C146" s="2">
-        <v>14513.618</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3">
+        <v>1085.4639999999999</v>
+      </c>
+      <c r="D146" s="2">
+        <v>3050.9180000000001</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
       <c r="A147" s="2">
         <v>202301</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C147" s="2">
-        <v>31489.677</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3">
+        <v>14513.618</v>
+      </c>
+      <c r="D147" s="2">
+        <v>106006.879</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
       <c r="A148" s="2">
         <v>202301</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C148" s="2">
-        <v>1085.4639999999999</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
+        <v>31489.677</v>
+      </c>
+      <c r="D148" s="2">
+        <v>143570.31899999999</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
       <c r="A149" s="2">
         <v>202302</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C149" s="2">
-        <v>14537.369000000001</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3">
+        <v>1067.866</v>
+      </c>
+      <c r="D149" s="2">
+        <v>2813.2289999999998</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
       <c r="A150" s="2">
         <v>202302</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C150" s="2">
-        <v>1067.866</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3">
+        <v>14537.369000000001</v>
+      </c>
+      <c r="D150" s="2">
+        <v>105564.37300000001</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
       <c r="A151" s="2">
         <v>202302</v>
       </c>
@@ -2119,74 +2573,95 @@
       <c r="C151" s="2">
         <v>32703.857</v>
       </c>
-    </row>
-    <row r="152" spans="1:3">
+      <c r="D151" s="2">
+        <v>146662.478</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
       <c r="A152" s="2">
         <v>202303</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C152" s="2">
-        <v>16443.021000000001</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
+        <v>1437.327</v>
+      </c>
+      <c r="D152" s="2">
+        <v>3377.5369999999998</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
       <c r="A153" s="2">
         <v>202303</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C153" s="2">
-        <v>37084.313000000002</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3">
+        <v>16443.021000000001</v>
+      </c>
+      <c r="D153" s="2">
+        <v>117751.011</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
       <c r="A154" s="2">
         <v>202303</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C154" s="2">
-        <v>1437.327</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3">
+        <v>37084.313000000002</v>
+      </c>
+      <c r="D154" s="2">
+        <v>164435.09700000001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
       <c r="A155" s="2">
         <v>202304</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C155" s="2">
-        <v>14446.065000000001</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
+        <v>1518.0239999999999</v>
+      </c>
+      <c r="D155" s="2">
+        <v>3498.0369999999998</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
       <c r="A156" s="2">
         <v>202304</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C156" s="2">
-        <v>32679.439999999999</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
+        <v>14446.065000000001</v>
+      </c>
+      <c r="D156" s="2">
+        <v>106743.86199999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
       <c r="A157" s="2">
         <v>202304</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C157" s="2">
-        <v>1518.0239999999999</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3">
+        <v>32679.439999999999</v>
+      </c>
+      <c r="D157" s="2">
+        <v>149029.92199999999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
       <c r="A158" s="2">
         <v>202305</v>
       </c>
@@ -2196,129 +2671,169 @@
       <c r="C158" s="2">
         <v>1419.24</v>
       </c>
-    </row>
-    <row r="159" spans="1:3">
+      <c r="D158" s="2">
+        <v>3234.6759999999999</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
       <c r="A159" s="2">
         <v>202305</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C159" s="2">
-        <v>34815.665999999997</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
+        <v>15266.925999999999</v>
+      </c>
+      <c r="D159" s="2">
+        <v>112991.239</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
       <c r="A160" s="2">
         <v>202305</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C160" s="2">
-        <v>15266.925999999999</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+        <v>34815.665999999997</v>
+      </c>
+      <c r="D160" s="2">
+        <v>157273.288</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161" s="2">
         <v>202306</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C161" s="2">
-        <v>14918.833000000001</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
+        <v>1339.5889999999999</v>
+      </c>
+      <c r="D161" s="2">
+        <v>2945.2330000000002</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162" s="2">
         <v>202306</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C162" s="2">
-        <v>34447.853000000003</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
+        <v>14918.833000000001</v>
+      </c>
+      <c r="D162" s="2">
+        <v>110988.356</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163" s="2">
         <v>202306</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C163" s="2">
-        <v>1339.5889999999999</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
+        <v>34447.853000000003</v>
+      </c>
+      <c r="D163" s="2">
+        <v>154532.87299999999</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164" s="2">
         <v>202307</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C164" s="2">
-        <v>15011.114</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+        <v>1704.7190000000001</v>
+      </c>
+      <c r="D164" s="2">
+        <v>3368.6210000000001</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165" s="2">
         <v>202307</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C165" s="2">
-        <v>35807.896999999997</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>15011.114</v>
+      </c>
+      <c r="D165" s="2">
+        <v>111344.713</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166" s="2">
         <v>202307</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C166" s="2">
-        <v>1704.7190000000001</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3">
+        <v>35807.896999999997</v>
+      </c>
+      <c r="D166" s="2">
+        <v>159913.83799999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167" s="2">
         <v>202308</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C167" s="2">
-        <v>15689.882</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+        <v>1858.4090000000001</v>
+      </c>
+      <c r="D167" s="2">
+        <v>3675.3960000000002</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168" s="2">
         <v>202308</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C168" s="2">
-        <v>37575.072</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
+        <v>15689.882</v>
+      </c>
+      <c r="D168" s="2">
+        <v>114501.084</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169" s="2">
         <v>202308</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C169" s="2">
-        <v>1858.4090000000001</v>
+        <v>37575.072</v>
+      </c>
+      <c r="D169" s="2">
+        <v>165155.15400000001</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D169">
+    <sortCondition ref="A2:A169"/>
+    <sortCondition ref="B2:B169"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>